<commit_message>
[Update] CodeBlockManager클래스 코드최적화 진행
</commit_message>
<xml_diff>
--- a/Assets/PSW/Excel/CodeBlockData.xlsx
+++ b/Assets/PSW/Excel/CodeBlockData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ViewName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,6 +34,38 @@
   </si>
   <si>
     <t>BlockName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Up</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Down</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Left</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Right</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackFire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackWater</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackGrass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Condition</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -359,15 +391,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.125" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="2" max="2" width="23.25" customWidth="1"/>
     <col min="3" max="3" width="12.375" customWidth="1"/>
     <col min="4" max="4" width="11.625" customWidth="1"/>
   </cols>
@@ -386,6 +419,70 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>